<commit_message>
Ready for CRAN - Since CRAN submission is not possible now - Added few features and tuning logics - Added more coverage
</commit_message>
<xml_diff>
--- a/inst/extdata/marks.xlsx
+++ b/inst/extdata/marks.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igayen\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igayen\Documents\RBI\WorkSpace\R_Packages\Stable\tidycells\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3308C30C-F1C2-4CA3-8F57-5DAB2BA9546A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{ACB3C22E-2C2A-49B3-9AAD-F7D7B5800ED3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>School A</t>
   </si>
@@ -76,9 +75,6 @@
   </si>
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Marks</t>
   </si>
   <si>
     <t>U Gupta</t>
@@ -96,7 +92,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -150,7 +146,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -173,23 +169,317 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,182 +793,193 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E06E6F7-845E-4A76-8413-C12CE1C81EEA}">
-  <dimension ref="A2:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="15">
+        <v>95</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="15">
+        <v>99</v>
+      </c>
+      <c r="E5" s="26" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1">
+        <v>50</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="15">
+        <v>89</v>
+      </c>
+      <c r="E6" s="27"/>
+      <c r="F6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="1">
+        <v>59</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16"/>
+      <c r="B7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="17">
+        <v>100</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1">
+        <v>61</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="28"/>
+      <c r="F8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="8">
+        <v>38</v>
+      </c>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="D11" s="19">
+        <v>70</v>
+      </c>
+      <c r="E11" s="19">
+        <v>75</v>
+      </c>
+      <c r="F11" s="19">
+        <v>81</v>
+      </c>
+      <c r="G11" s="20">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="2"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2">
-        <v>95</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2">
-        <v>50</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2">
-        <v>99</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2">
-        <v>59</v>
-      </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="E13" s="24"/>
+      <c r="F13" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2">
-        <v>89</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="2">
-        <v>61</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2">
-        <v>100</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="2">
-        <v>38</v>
-      </c>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="6">
-        <v>70</v>
-      </c>
-      <c r="E11" s="6">
-        <v>75</v>
-      </c>
-      <c r="F11" s="6">
-        <v>81</v>
-      </c>
-      <c r="G11" s="6">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="4"/>
+      <c r="G13" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="E5:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>